<commit_message>
Cambio a còdigo climatico
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\paquetes\clima\clima\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Phyton\clima\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Identificador</t>
   </si>
@@ -63,6 +63,27 @@
   </si>
   <si>
     <t>Modbus_Ala</t>
+  </si>
+  <si>
+    <t>Esmeraldas,EC</t>
+  </si>
+  <si>
+    <t>Manta,EC</t>
+  </si>
+  <si>
+    <t>Santo Domingo,EC</t>
+  </si>
+  <si>
+    <t>Machala,EC</t>
+  </si>
+  <si>
+    <t>Puyo,EC</t>
+  </si>
+  <si>
+    <t>Tena,EC</t>
+  </si>
+  <si>
+    <t>Macas,EC</t>
   </si>
 </sst>
 </file>
@@ -389,16 +410,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="E9" sqref="E9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
@@ -447,8 +468,8 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <f>C2+4</f>
-        <v>30496</v>
+        <f>C2+2</f>
+        <v>30494</v>
       </c>
       <c r="D3">
         <f>D2+1</f>
@@ -460,18 +481,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+        <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="1">C3+4</f>
-        <v>30500</v>
+        <f t="shared" ref="C4:C15" si="1">C3+2</f>
+        <v>30496</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D8" si="2">D3+1</f>
+        <f t="shared" ref="D4:D15" si="2">D3+1</f>
         <v>20498</v>
       </c>
       <c r="E4" t="s">
@@ -488,7 +509,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>30504</v>
+        <v>30498</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
@@ -508,7 +529,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>30508</v>
+        <v>30500</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
@@ -528,7 +549,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>30512</v>
+        <v>30502</v>
       </c>
       <c r="D7">
         <v>20502</v>
@@ -547,13 +568,153 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
+        <v>30504</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>20503</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>30506</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>20504</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>30508</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>20505</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>30510</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>20506</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>30512</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>20507</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>30514</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>20508</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
         <v>30516</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>20503</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>20509</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>30518</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>20510</v>
+      </c>
+      <c r="E15" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio a còdigo climatico y temperatura
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Phyton\clima\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Phyton\clima2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Identificador</t>
   </si>
@@ -32,58 +32,67 @@
     <t>Ciudad</t>
   </si>
   <si>
-    <t>Modbus_Add</t>
-  </si>
-  <si>
     <t>Activa</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
+    <t>Cuenca, EC</t>
+  </si>
+  <si>
+    <t>Riobamba, EC</t>
+  </si>
+  <si>
+    <t>Tulcan, EC</t>
+  </si>
+  <si>
+    <t>Guayaquil,EC</t>
+  </si>
+  <si>
+    <t>Quito, EC</t>
+  </si>
+  <si>
+    <t>Modbus_Ala</t>
+  </si>
+  <si>
+    <t>Esmeraldas,EC</t>
+  </si>
+  <si>
+    <t>Manta,EC</t>
+  </si>
+  <si>
+    <t>Machala,EC</t>
+  </si>
+  <si>
+    <t>Puyo,EC</t>
+  </si>
+  <si>
+    <t>Tena,EC</t>
+  </si>
+  <si>
+    <t>Macas,EC</t>
+  </si>
+  <si>
+    <t>Modbus_Add_wc</t>
+  </si>
+  <si>
+    <t>Modbus_Add_temp</t>
+  </si>
+  <si>
+    <t>EMS_cod</t>
+  </si>
+  <si>
+    <t>EMS_temp</t>
+  </si>
+  <si>
     <t>Portoviejo, EC</t>
   </si>
   <si>
-    <t>Cuenca, EC</t>
-  </si>
-  <si>
     <t>Latacunga, EC</t>
   </si>
   <si>
-    <t>Riobamba, EC</t>
-  </si>
-  <si>
-    <t>Tulcan, EC</t>
-  </si>
-  <si>
-    <t>Guayaquil,EC</t>
-  </si>
-  <si>
-    <t>Quito, EC</t>
-  </si>
-  <si>
-    <t>Modbus_Ala</t>
-  </si>
-  <si>
-    <t>Esmeraldas,EC</t>
-  </si>
-  <si>
-    <t>Manta,EC</t>
-  </si>
-  <si>
-    <t>Santo Domingo,EC</t>
-  </si>
-  <si>
-    <t>Machala,EC</t>
-  </si>
-  <si>
-    <t>Puyo,EC</t>
-  </si>
-  <si>
-    <t>Tena,EC</t>
-  </si>
-  <si>
-    <t>Macas,EC</t>
+    <t>Loja,EC</t>
   </si>
 </sst>
 </file>
@@ -410,21 +419,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E15"/>
+      <selection activeCell="H3" sqref="H3:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,290 +442,464 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>30492</v>
       </c>
       <c r="D2">
+        <v>31548</v>
+      </c>
+      <c r="E2">
         <v>20496</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>C2+2</f>
         <v>30494</v>
       </c>
       <c r="D3">
-        <f>D2+1</f>
+        <f>D2+2</f>
+        <v>31550</v>
+      </c>
+      <c r="E3">
+        <f>E2+1</f>
         <v>20497</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>G2+1</f>
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <f>H2+1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C15" si="1">C3+2</f>
+        <f t="shared" ref="C4:D15" si="1">C3+2</f>
         <v>30496</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D15" si="2">D3+1</f>
+        <f t="shared" si="1"/>
+        <v>31552</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="2">E3+1</f>
         <v>20498</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:H15" si="3">G3+1</f>
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
         <v>30498</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>31554</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="2"/>
         <v>20499</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
         <v>30500</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>31556</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="2"/>
         <v>20500</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
         <v>30502</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>31558</v>
+      </c>
+      <c r="E7">
         <v>20502</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
         <v>30504</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>31560</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="2"/>
         <v>20503</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
         <v>30506</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>31562</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="2"/>
         <v>20504</v>
       </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
         <v>30508</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>31564</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
         <v>20505</v>
       </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
         <v>30510</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>31566</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="2"/>
         <v>20506</v>
       </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
         <v>30512</v>
       </c>
       <c r="D12">
+        <f t="shared" si="1"/>
+        <v>31568</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="2"/>
         <v>20507</v>
       </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
         <v>30514</v>
       </c>
       <c r="D13">
+        <f t="shared" si="1"/>
+        <v>31570</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="2"/>
         <v>20508</v>
       </c>
-      <c r="E13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
         <v>30516</v>
       </c>
       <c r="D14">
+        <f t="shared" si="1"/>
+        <v>31572</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="2"/>
         <v>20509</v>
       </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
         <v>30518</v>
       </c>
       <c r="D15">
+        <f t="shared" si="1"/>
+        <v>31574</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="2"/>
         <v>20510</v>
       </c>
-      <c r="E15" t="s">
-        <v>4</v>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>